<commit_message>
corrige dados. altera gráficos de barra.
</commit_message>
<xml_diff>
--- a/dados/Estatais_rev2.xlsx
+++ b/dados/Estatais_rev2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\estatais-estados\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1095E37-538E-4C23-9938-47C4D4C204AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2467A53D-8A72-4319-8F45-6E93D498C84A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6676EBA9-1B60-4743-AD0B-38828D275A1F}"/>
   </bookViews>
@@ -33,8 +33,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId12"/>
-    <pivotCache cacheId="26" r:id="rId13"/>
+    <pivotCache cacheId="29" r:id="rId12"/>
+    <pivotCache cacheId="30" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="426">
   <si>
     <t>Estado</t>
   </si>
@@ -1510,9 +1510,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Não Declarado</t>
   </si>
 </sst>
@@ -1772,6 +1769,12 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -1804,12 +1807,6 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -43442,7 +43439,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF3CD36F-AD9C-474D-82A4-4FEB4C47B334}" name="Tabela dinâmica2" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF3CD36F-AD9C-474D-82A4-4FEB4C47B334}" name="Tabela dinâmica2" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" sortType="descending">
@@ -43602,7 +43599,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61B1AD8F-02E7-40CB-A1FE-5E24D85FA955}" name="Tabela dinâmica1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61B1AD8F-02E7-40CB-A1FE-5E24D85FA955}" name="Tabela dinâmica1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:A76" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -44173,7 +44170,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D376FFE4-9E01-440D-A89A-0615558CD5CD}" name="Tabela dinâmica1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D376FFE4-9E01-440D-A89A-0615558CD5CD}" name="Tabela dinâmica1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0">
@@ -44598,7 +44595,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{108DFA18-215C-48DD-A8FA-0184EDE7DC13}" name="Tabela dinâmica3" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{108DFA18-215C-48DD-A8FA-0184EDE7DC13}" name="Tabela dinâmica3" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B28:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0">
@@ -45009,7 +45006,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54178E12-E6C4-40BF-B68F-A0C0C4BF1E6E}" name="Tabela dinâmica2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54178E12-E6C4-40BF-B68F-A0C0C4BF1E6E}" name="Tabela dinâmica2" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="C3:F31" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -45615,10 +45612,10 @@
     <dataField name="Soma de Reforço de Capital" fld="10" baseField="0" baseItem="2"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="7">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="1">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -45641,7 +45638,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5126215-D479-4739-AB6F-A45F3724CC30}" name="Tabela dinâmica1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5126215-D479-4739-AB6F-A45F3724CC30}" name="Tabela dinâmica1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:B32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
@@ -46117,11 +46114,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEE7169-4F29-4161-8BCE-CD1E6900F234}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:N261"/>
+  <dimension ref="A1:N259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46487,7 +46484,7 @@
         <v>24</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -46515,7 +46512,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -46543,7 +46540,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -46640,7 +46637,7 @@
         <v>29</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H15" s="4">
         <v>5650868</v>
@@ -46670,7 +46667,7 @@
         <v>30</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -46699,7 +46696,7 @@
         <v>31</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H17" s="4">
         <v>6721921.4699999997</v>
@@ -46966,7 +46963,7 @@
         <v>27</v>
       </c>
       <c r="G25" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -46993,7 +46990,7 @@
         <v>66</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -50150,7 +50147,7 @@
         <v>26</v>
       </c>
       <c r="G121" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H121" s="4">
         <v>12980955.85</v>
@@ -50620,7 +50617,7 @@
         <v>29</v>
       </c>
       <c r="G134" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
@@ -50645,13 +50642,13 @@
         <v>349</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>425</v>
+        <v>349</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G135" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H135" s="4">
         <v>48597738.68</v>
@@ -50725,7 +50722,7 @@
         <v>49</v>
       </c>
       <c r="G137" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H137" s="4">
         <v>7508717.0499999998</v>
@@ -50795,7 +50792,7 @@
         <v>223</v>
       </c>
       <c r="G139" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H139" s="4">
         <v>21309325.030000001</v>
@@ -51387,7 +51384,7 @@
         <v>28</v>
       </c>
       <c r="G156" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J156" s="4"/>
       <c r="K156" s="4"/>
@@ -51414,7 +51411,7 @@
         <v>66</v>
       </c>
       <c r="G157" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H157" s="4">
         <v>-852906000</v>
@@ -51447,7 +51444,7 @@
         <v>27</v>
       </c>
       <c r="G158" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
@@ -51467,6 +51464,9 @@
       <c r="D159" s="2" t="s">
         <v>349</v>
       </c>
+      <c r="E159" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="F159" s="2" t="s">
         <v>23</v>
       </c>
@@ -51504,7 +51504,7 @@
         <v>29</v>
       </c>
       <c r="G160" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
@@ -51531,7 +51531,7 @@
         <v>29</v>
       </c>
       <c r="G161" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J161" s="4"/>
       <c r="K161" s="4"/>
@@ -51558,7 +51558,7 @@
         <v>65</v>
       </c>
       <c r="G162" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J162" s="4"/>
       <c r="K162" s="4"/>
@@ -51585,7 +51585,7 @@
         <v>402</v>
       </c>
       <c r="G163" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
@@ -51612,7 +51612,7 @@
         <v>24</v>
       </c>
       <c r="G164" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J164" s="4"/>
       <c r="K164" s="4"/>
@@ -52008,7 +52008,7 @@
         <v>29</v>
       </c>
       <c r="G176" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H176" s="4">
         <v>-301434356</v>
@@ -52234,7 +52234,7 @@
         <v>47</v>
       </c>
       <c r="G182" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H182" s="4">
         <v>-401510.53</v>
@@ -52344,7 +52344,7 @@
         <v>27</v>
       </c>
       <c r="G185" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H185" s="4" t="s">
         <v>411</v>
@@ -52552,7 +52552,7 @@
         <v>27</v>
       </c>
       <c r="G191" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H191" s="4">
         <v>693724435.88000023</v>
@@ -52772,7 +52772,7 @@
         <v>401</v>
       </c>
       <c r="G198" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H198" s="4">
         <v>1843606621.1900001</v>
@@ -52804,7 +52804,7 @@
         <v>23</v>
       </c>
       <c r="G199" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H199" s="12">
         <v>228626667.16999999</v>
@@ -52834,7 +52834,7 @@
         <v>27</v>
       </c>
       <c r="G200" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H200" s="4">
         <v>-322334000</v>
@@ -52864,7 +52864,7 @@
         <v>23</v>
       </c>
       <c r="G201" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J201" s="4"/>
       <c r="K201" s="4"/>
@@ -53016,7 +53016,7 @@
         <v>47</v>
       </c>
       <c r="G206" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H206" s="4">
         <v>0</v>
@@ -53868,7 +53868,7 @@
         <v>23</v>
       </c>
       <c r="G232" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H232" s="4">
         <v>-641580.82999999996</v>
@@ -54795,7 +54795,7 @@
         <v>65822000</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>193</v>
       </c>
@@ -54825,7 +54825,7 @@
       <c r="L257" s="4"/>
       <c r="M257" s="4"/>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>193</v>
       </c>
@@ -54855,7 +54855,7 @@
       <c r="L258" s="4"/>
       <c r="M258" s="4"/>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>193</v>
       </c>
@@ -54887,48 +54887,25 @@
         <v>185000</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H260" s="4"/>
-      <c r="I260" s="4"/>
-      <c r="J260" s="31"/>
-      <c r="K260" s="31"/>
-      <c r="L260" s="31"/>
-      <c r="M260" s="31"/>
-      <c r="N260" s="31"/>
-    </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J261" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K261" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L261" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M261" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:D31 B32:C32 B33:D1048576">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Não tem Quadro">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Não tem Quadro">
       <formula>NOT(ISERROR(SEARCH("Não tem Quadro",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B185:D185">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Não tem Quadro">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Não tem Quadro">
       <formula>NOT(ISERROR(SEARCH("Não tem Quadro",B185)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B223">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="SANEAMENTO">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="SANEAMENTO">
       <formula>NOT(ISERROR(SEARCH("SANEAMENTO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Esgoto">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Esgoto">
       <formula>NOT(ISERROR(SEARCH("Esgoto",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="água">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="água">
       <formula>NOT(ISERROR(SEARCH("água",B7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>